<commit_message>
Working on user interface
</commit_message>
<xml_diff>
--- a/cs_csvtings/..\..\..\my_employees.xlsx
+++ b/cs_csvtings/..\..\..\my_employees.xlsx
@@ -52,85 +52,85 @@
     <x:t>Project Manager</x:t>
   </x:si>
   <x:si>
+    <x:t>jane.smith@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mike Brown</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quality Assurance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mike.brown@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sarah Miller</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UI/UX Designer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Design</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sarah.miller@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Olivia Jones</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Analyst</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Science</x:t>
+  </x:si>
+  <x:si>
+    <x:t>olivia.jones@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daniel Garcia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sales Representative</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sales</x:t>
+  </x:si>
+  <x:si>
+    <x:t>daniel.garcia@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Emma Wilson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HR Specialist</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Human Resources</x:t>
+  </x:si>
+  <x:si>
+    <x:t>emma.wilson@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Carlos Sanchez</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer Support</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Support</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carlos.sanchez@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sophia Davis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marketing Coordinator</x:t>
+  </x:si>
+  <x:si>
     <x:t>Marketing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>jane.smith@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mike Brown</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Quality Assurance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mike.brown@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sarah Miller</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UI/UX Designer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Design</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sarah.miller@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Olivia Jones</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Data Analyst</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Data Science</x:t>
-  </x:si>
-  <x:si>
-    <x:t>olivia.jones@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daniel Garcia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sales Representative</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sales</x:t>
-  </x:si>
-  <x:si>
-    <x:t>daniel.garcia@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Emma Wilson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HR Specialist</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Human Resources</x:t>
-  </x:si>
-  <x:si>
-    <x:t>emma.wilson@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Carlos Sanchez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Customer Support</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Support</x:t>
-  </x:si>
-  <x:si>
-    <x:t>carlos.sanchez@example.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sophia Davis</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Marketing Coordinator</x:t>
   </x:si>
   <x:si>
     <x:t>sophia.davis@example.com</x:t>
@@ -553,13 +553,13 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D3" s="0">
-        <x:v>0</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
         <x:v>12</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6">
@@ -567,10 +567,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>15</x:v>
       </x:c>
       <x:c r="D4" s="0">
         <x:v>0</x:v>
@@ -579,7 +579,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
@@ -587,19 +587,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="D5" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D5" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
+      <x:c r="F5" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
@@ -607,19 +607,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D6" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
+      <x:c r="F6" s="0" t="s">
         <x:v>23</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
@@ -627,19 +627,19 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="D7" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="D7" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
+      <x:c r="F7" s="0" t="s">
         <x:v>27</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
@@ -647,19 +647,19 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
+      <x:c r="D8" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D8" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
+      <x:c r="F8" s="0" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="F8" s="0" t="s">
-        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
@@ -667,19 +667,19 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C9" s="0" t="s">
+      <x:c r="D9" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D9" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
+      <x:c r="F9" s="0" t="s">
         <x:v>35</x:v>
-      </x:c>
-      <x:c r="F9" s="0" t="s">
-        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
@@ -687,16 +687,16 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C10" s="0" t="s">
+      <x:c r="D10" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
         <x:v>38</x:v>
-      </x:c>
-      <x:c r="D10" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>12</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
         <x:v>39</x:v>

</xml_diff>